<commit_message>
Added method to create a new takeoff.
</commit_message>
<xml_diff>
--- a/TAKEOFF CONCEPT.xlsx
+++ b/TAKEOFF CONCEPT.xlsx
@@ -2860,7 +2860,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="100">
   <si>
     <t>MK</t>
   </si>
@@ -3176,22 +3176,55 @@
     <t>4</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>LOAD NOTE</t>
   </si>
   <si>
     <t>JOIST REMARKS</t>
   </si>
   <si>
-    <t>WH</t>
+    <t>Load Note</t>
   </si>
   <si>
-    <t>Load Note</t>
+    <t>BRACE</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>32LH300/150</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>DL</t>
   </si>
 </sst>
 </file>
@@ -4545,105 +4578,8 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" indent="6"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4652,81 +4588,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -4742,15 +4608,216 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="166" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="52" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4760,41 +4827,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4806,46 +4879,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5159,82 +5192,82 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="163" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142"/>
-      <c r="M1" s="142"/>
-      <c r="N1" s="142"/>
-      <c r="O1" s="142"/>
-      <c r="P1" s="142"/>
-      <c r="Q1" s="142"/>
-      <c r="R1" s="142"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="115"/>
+      <c r="M1" s="115"/>
+      <c r="N1" s="115"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
       <c r="H2" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="136" t="s">
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="136"/>
-      <c r="O2" s="148" t="s">
+      <c r="N2" s="108"/>
+      <c r="O2" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="166"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="121"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="135" t="s">
+      <c r="A3" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="153" t="s">
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="153"/>
-      <c r="F3" s="153"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="153"/>
-      <c r="I3" s="153"/>
-      <c r="J3" s="153"/>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="136" t="s">
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="136"/>
-      <c r="O3" s="158" t="s">
+      <c r="N3" s="108"/>
+      <c r="O3" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="158"/>
+      <c r="P3" s="110"/>
       <c r="Q3" s="57" t="s">
         <v>39</v>
       </c>
@@ -5243,102 +5276,102 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="135" t="s">
+      <c r="A4" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="136"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="153" t="s">
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="153"/>
-      <c r="H4" s="153"/>
-      <c r="I4" s="153"/>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="153"/>
-      <c r="M4" s="136" t="s">
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="136"/>
-      <c r="O4" s="153" t="s">
+      <c r="N4" s="108"/>
+      <c r="O4" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="153"/>
-      <c r="Q4" s="153"/>
-      <c r="R4" s="160"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="111"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="135" t="s">
+      <c r="A5" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="153" t="s">
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="153"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="153"/>
-      <c r="L5" s="153"/>
-      <c r="M5" s="136" t="s">
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="136"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="136"/>
-      <c r="Q5" s="137" t="s">
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="138"/>
+      <c r="R5" s="127"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="154"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="153"/>
-      <c r="E6" s="153"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153"/>
-      <c r="I6" s="153"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="153"/>
-      <c r="M6" s="136" t="s">
+      <c r="A6" s="128"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="136"/>
-      <c r="O6" s="136"/>
-      <c r="P6" s="136"/>
-      <c r="Q6" s="158" t="s">
+      <c r="N6" s="108"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="159"/>
+      <c r="R6" s="132"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="156"/>
-      <c r="B7" s="157"/>
-      <c r="C7" s="157"/>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="136" t="s">
+      <c r="A7" s="130"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="136"/>
+      <c r="N7" s="108"/>
       <c r="O7" s="59">
         <v>1</v>
       </c>
@@ -5351,644 +5384,644 @@
       <c r="R7" s="61"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="146" t="s">
+      <c r="A8" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="147"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="148" t="s">
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="148"/>
-      <c r="F8" s="148"/>
-      <c r="G8" s="147" t="s">
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="147"/>
-      <c r="I8" s="149" t="s">
+      <c r="H8" s="122"/>
+      <c r="I8" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="149"/>
-      <c r="K8" s="147" t="s">
+      <c r="J8" s="118"/>
+      <c r="K8" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="147"/>
-      <c r="M8" s="150" t="s">
+      <c r="L8" s="122"/>
+      <c r="M8" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="151"/>
-      <c r="O8" s="151"/>
-      <c r="P8" s="151"/>
-      <c r="Q8" s="151"/>
-      <c r="R8" s="152"/>
+      <c r="N8" s="124"/>
+      <c r="O8" s="124"/>
+      <c r="P8" s="124"/>
+      <c r="Q8" s="124"/>
+      <c r="R8" s="125"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="135" t="s">
+      <c r="A9" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="136"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="137" t="s">
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="136" t="s">
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="136"/>
-      <c r="I9" s="137" t="s">
+      <c r="H9" s="108"/>
+      <c r="I9" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="137"/>
-      <c r="K9" s="136" t="s">
+      <c r="J9" s="126"/>
+      <c r="K9" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="136"/>
-      <c r="M9" s="137" t="s">
+      <c r="L9" s="108"/>
+      <c r="M9" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="144"/>
-      <c r="O9" s="144"/>
-      <c r="P9" s="144"/>
-      <c r="Q9" s="144"/>
-      <c r="R9" s="145"/>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
+      <c r="P9" s="137"/>
+      <c r="Q9" s="137"/>
+      <c r="R9" s="138"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="135" t="s">
+      <c r="A10" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="136"/>
-      <c r="C10" s="136"/>
-      <c r="D10" s="137" t="s">
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="126" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="137"/>
-      <c r="F10" s="137"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="137"/>
-      <c r="J10" s="137"/>
-      <c r="K10" s="137"/>
-      <c r="L10" s="137"/>
-      <c r="M10" s="137"/>
-      <c r="N10" s="137"/>
-      <c r="O10" s="137"/>
-      <c r="P10" s="137"/>
-      <c r="Q10" s="137"/>
-      <c r="R10" s="138"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="126"/>
+      <c r="K10" s="126"/>
+      <c r="L10" s="126"/>
+      <c r="M10" s="126"/>
+      <c r="N10" s="126"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
+      <c r="R10" s="127"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="139"/>
-      <c r="B11" s="140"/>
-      <c r="C11" s="140"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="137"/>
-      <c r="P11" s="137"/>
-      <c r="Q11" s="137"/>
-      <c r="R11" s="138"/>
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="126"/>
+      <c r="O11" s="126"/>
+      <c r="P11" s="126"/>
+      <c r="Q11" s="126"/>
+      <c r="R11" s="127"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="135" t="s">
+      <c r="A12" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="141" t="s">
+      <c r="B12" s="108"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="141"/>
-      <c r="F12" s="141"/>
-      <c r="G12" s="141"/>
-      <c r="H12" s="141"/>
-      <c r="I12" s="141"/>
-      <c r="J12" s="141"/>
-      <c r="K12" s="142"/>
-      <c r="L12" s="142"/>
-      <c r="M12" s="142"/>
-      <c r="N12" s="142"/>
-      <c r="O12" s="142"/>
-      <c r="P12" s="142"/>
-      <c r="Q12" s="142"/>
-      <c r="R12" s="143"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="115"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="115"/>
+      <c r="P12" s="115"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="136"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="127" t="s">
+      <c r="A13" s="142" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="128"/>
-      <c r="C13" s="129" t="s">
+      <c r="B13" s="143"/>
+      <c r="C13" s="144" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="130"/>
-      <c r="G13" s="130"/>
-      <c r="H13" s="130"/>
-      <c r="I13" s="130"/>
-      <c r="J13" s="130"/>
-      <c r="K13" s="130"/>
-      <c r="L13" s="130"/>
-      <c r="M13" s="130"/>
-      <c r="N13" s="130"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="130"/>
-      <c r="Q13" s="130"/>
-      <c r="R13" s="131"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="145"/>
+      <c r="H13" s="145"/>
+      <c r="I13" s="145"/>
+      <c r="J13" s="145"/>
+      <c r="K13" s="145"/>
+      <c r="L13" s="145"/>
+      <c r="M13" s="145"/>
+      <c r="N13" s="145"/>
+      <c r="O13" s="145"/>
+      <c r="P13" s="145"/>
+      <c r="Q13" s="145"/>
+      <c r="R13" s="146"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
-      <c r="B14" s="132"/>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="133"/>
-      <c r="O14" s="133"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="134"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="148"/>
+      <c r="D14" s="148"/>
+      <c r="E14" s="148"/>
+      <c r="F14" s="148"/>
+      <c r="G14" s="148"/>
+      <c r="H14" s="148"/>
+      <c r="I14" s="148"/>
+      <c r="J14" s="148"/>
+      <c r="K14" s="148"/>
+      <c r="L14" s="148"/>
+      <c r="M14" s="148"/>
+      <c r="N14" s="148"/>
+      <c r="O14" s="148"/>
+      <c r="P14" s="148"/>
+      <c r="Q14" s="148"/>
+      <c r="R14" s="149"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="63"/>
-      <c r="B15" s="124"/>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="125"/>
-      <c r="H15" s="125"/>
-      <c r="I15" s="125"/>
-      <c r="J15" s="125"/>
-      <c r="K15" s="125"/>
-      <c r="L15" s="125"/>
-      <c r="M15" s="125"/>
-      <c r="N15" s="125"/>
-      <c r="O15" s="125"/>
-      <c r="P15" s="125"/>
-      <c r="Q15" s="125"/>
-      <c r="R15" s="126"/>
+      <c r="B15" s="139"/>
+      <c r="C15" s="140"/>
+      <c r="D15" s="140"/>
+      <c r="E15" s="140"/>
+      <c r="F15" s="140"/>
+      <c r="G15" s="140"/>
+      <c r="H15" s="140"/>
+      <c r="I15" s="140"/>
+      <c r="J15" s="140"/>
+      <c r="K15" s="140"/>
+      <c r="L15" s="140"/>
+      <c r="M15" s="140"/>
+      <c r="N15" s="140"/>
+      <c r="O15" s="140"/>
+      <c r="P15" s="140"/>
+      <c r="Q15" s="140"/>
+      <c r="R15" s="141"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="63"/>
-      <c r="B16" s="124"/>
-      <c r="C16" s="125"/>
-      <c r="D16" s="125"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="125"/>
-      <c r="I16" s="125"/>
-      <c r="J16" s="125"/>
-      <c r="K16" s="125"/>
-      <c r="L16" s="125"/>
-      <c r="M16" s="125"/>
-      <c r="N16" s="125"/>
-      <c r="O16" s="125"/>
-      <c r="P16" s="125"/>
-      <c r="Q16" s="125"/>
-      <c r="R16" s="126"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="140"/>
+      <c r="D16" s="140"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="140"/>
+      <c r="I16" s="140"/>
+      <c r="J16" s="140"/>
+      <c r="K16" s="140"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="140"/>
+      <c r="P16" s="140"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="141"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="63"/>
-      <c r="B17" s="124"/>
-      <c r="C17" s="125"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="125"/>
-      <c r="G17" s="125"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="125"/>
-      <c r="J17" s="125"/>
-      <c r="K17" s="125"/>
-      <c r="L17" s="125"/>
-      <c r="M17" s="125"/>
-      <c r="N17" s="125"/>
-      <c r="O17" s="125"/>
-      <c r="P17" s="125"/>
-      <c r="Q17" s="125"/>
-      <c r="R17" s="126"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="140"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="140"/>
+      <c r="I17" s="140"/>
+      <c r="J17" s="140"/>
+      <c r="K17" s="140"/>
+      <c r="L17" s="140"/>
+      <c r="M17" s="140"/>
+      <c r="N17" s="140"/>
+      <c r="O17" s="140"/>
+      <c r="P17" s="140"/>
+      <c r="Q17" s="140"/>
+      <c r="R17" s="141"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="63"/>
-      <c r="B18" s="124"/>
-      <c r="C18" s="125"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="125"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="125"/>
-      <c r="M18" s="125"/>
-      <c r="N18" s="125"/>
-      <c r="O18" s="125"/>
-      <c r="P18" s="125"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="126"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="140"/>
+      <c r="D18" s="140"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="140"/>
+      <c r="I18" s="140"/>
+      <c r="J18" s="140"/>
+      <c r="K18" s="140"/>
+      <c r="L18" s="140"/>
+      <c r="M18" s="140"/>
+      <c r="N18" s="140"/>
+      <c r="O18" s="140"/>
+      <c r="P18" s="140"/>
+      <c r="Q18" s="140"/>
+      <c r="R18" s="141"/>
     </row>
     <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="63"/>
-      <c r="B19" s="124"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="125"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="125"/>
-      <c r="N19" s="125"/>
-      <c r="O19" s="125"/>
-      <c r="P19" s="125"/>
-      <c r="Q19" s="125"/>
-      <c r="R19" s="126"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="140"/>
+      <c r="I19" s="140"/>
+      <c r="J19" s="140"/>
+      <c r="K19" s="140"/>
+      <c r="L19" s="140"/>
+      <c r="M19" s="140"/>
+      <c r="N19" s="140"/>
+      <c r="O19" s="140"/>
+      <c r="P19" s="140"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="141"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="63"/>
-      <c r="B20" s="124"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="125"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="125"/>
-      <c r="K20" s="125"/>
-      <c r="L20" s="125"/>
-      <c r="M20" s="125"/>
-      <c r="N20" s="125"/>
-      <c r="O20" s="125"/>
-      <c r="P20" s="125"/>
-      <c r="Q20" s="125"/>
-      <c r="R20" s="126"/>
+      <c r="B20" s="139"/>
+      <c r="C20" s="140"/>
+      <c r="D20" s="140"/>
+      <c r="E20" s="140"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="140"/>
+      <c r="H20" s="140"/>
+      <c r="I20" s="140"/>
+      <c r="J20" s="140"/>
+      <c r="K20" s="140"/>
+      <c r="L20" s="140"/>
+      <c r="M20" s="140"/>
+      <c r="N20" s="140"/>
+      <c r="O20" s="140"/>
+      <c r="P20" s="140"/>
+      <c r="Q20" s="140"/>
+      <c r="R20" s="141"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="63"/>
-      <c r="B21" s="124"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="125"/>
-      <c r="F21" s="125"/>
-      <c r="G21" s="125"/>
-      <c r="H21" s="125"/>
-      <c r="I21" s="125"/>
-      <c r="J21" s="125"/>
-      <c r="K21" s="125"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
-      <c r="N21" s="125"/>
-      <c r="O21" s="125"/>
-      <c r="P21" s="125"/>
-      <c r="Q21" s="125"/>
-      <c r="R21" s="126"/>
+      <c r="B21" s="139"/>
+      <c r="C21" s="140"/>
+      <c r="D21" s="140"/>
+      <c r="E21" s="140"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="140"/>
+      <c r="I21" s="140"/>
+      <c r="J21" s="140"/>
+      <c r="K21" s="140"/>
+      <c r="L21" s="140"/>
+      <c r="M21" s="140"/>
+      <c r="N21" s="140"/>
+      <c r="O21" s="140"/>
+      <c r="P21" s="140"/>
+      <c r="Q21" s="140"/>
+      <c r="R21" s="141"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="63"/>
-      <c r="B22" s="124"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125"/>
-      <c r="F22" s="125"/>
-      <c r="G22" s="125"/>
-      <c r="H22" s="125"/>
-      <c r="I22" s="125"/>
-      <c r="J22" s="125"/>
-      <c r="K22" s="125"/>
-      <c r="L22" s="125"/>
-      <c r="M22" s="125"/>
-      <c r="N22" s="125"/>
-      <c r="O22" s="125"/>
-      <c r="P22" s="125"/>
-      <c r="Q22" s="125"/>
-      <c r="R22" s="126"/>
+      <c r="B22" s="139"/>
+      <c r="C22" s="140"/>
+      <c r="D22" s="140"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="140"/>
+      <c r="I22" s="140"/>
+      <c r="J22" s="140"/>
+      <c r="K22" s="140"/>
+      <c r="L22" s="140"/>
+      <c r="M22" s="140"/>
+      <c r="N22" s="140"/>
+      <c r="O22" s="140"/>
+      <c r="P22" s="140"/>
+      <c r="Q22" s="140"/>
+      <c r="R22" s="141"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="63"/>
-      <c r="B23" s="124"/>
-      <c r="C23" s="125"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="125"/>
-      <c r="G23" s="125"/>
-      <c r="H23" s="125"/>
-      <c r="I23" s="125"/>
-      <c r="J23" s="125"/>
-      <c r="K23" s="125"/>
-      <c r="L23" s="125"/>
-      <c r="M23" s="125"/>
-      <c r="N23" s="125"/>
-      <c r="O23" s="125"/>
-      <c r="P23" s="125"/>
-      <c r="Q23" s="125"/>
-      <c r="R23" s="126"/>
+      <c r="B23" s="139"/>
+      <c r="C23" s="140"/>
+      <c r="D23" s="140"/>
+      <c r="E23" s="140"/>
+      <c r="F23" s="140"/>
+      <c r="G23" s="140"/>
+      <c r="H23" s="140"/>
+      <c r="I23" s="140"/>
+      <c r="J23" s="140"/>
+      <c r="K23" s="140"/>
+      <c r="L23" s="140"/>
+      <c r="M23" s="140"/>
+      <c r="N23" s="140"/>
+      <c r="O23" s="140"/>
+      <c r="P23" s="140"/>
+      <c r="Q23" s="140"/>
+      <c r="R23" s="141"/>
     </row>
     <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="63"/>
-      <c r="B24" s="124"/>
-      <c r="C24" s="125"/>
-      <c r="D24" s="125"/>
-      <c r="E24" s="125"/>
-      <c r="F24" s="125"/>
-      <c r="G24" s="125"/>
-      <c r="H24" s="125"/>
-      <c r="I24" s="125"/>
-      <c r="J24" s="125"/>
-      <c r="K24" s="125"/>
-      <c r="L24" s="125"/>
-      <c r="M24" s="125"/>
-      <c r="N24" s="125"/>
-      <c r="O24" s="125"/>
-      <c r="P24" s="125"/>
-      <c r="Q24" s="125"/>
-      <c r="R24" s="126"/>
+      <c r="B24" s="139"/>
+      <c r="C24" s="140"/>
+      <c r="D24" s="140"/>
+      <c r="E24" s="140"/>
+      <c r="F24" s="140"/>
+      <c r="G24" s="140"/>
+      <c r="H24" s="140"/>
+      <c r="I24" s="140"/>
+      <c r="J24" s="140"/>
+      <c r="K24" s="140"/>
+      <c r="L24" s="140"/>
+      <c r="M24" s="140"/>
+      <c r="N24" s="140"/>
+      <c r="O24" s="140"/>
+      <c r="P24" s="140"/>
+      <c r="Q24" s="140"/>
+      <c r="R24" s="141"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="63"/>
-      <c r="B25" s="124"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="125"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="125"/>
-      <c r="G25" s="125"/>
-      <c r="H25" s="125"/>
-      <c r="I25" s="125"/>
-      <c r="J25" s="125"/>
-      <c r="K25" s="125"/>
-      <c r="L25" s="125"/>
-      <c r="M25" s="125"/>
-      <c r="N25" s="125"/>
-      <c r="O25" s="125"/>
-      <c r="P25" s="125"/>
-      <c r="Q25" s="125"/>
-      <c r="R25" s="126"/>
+      <c r="B25" s="139"/>
+      <c r="C25" s="140"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="140"/>
+      <c r="F25" s="140"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="140"/>
+      <c r="I25" s="140"/>
+      <c r="J25" s="140"/>
+      <c r="K25" s="140"/>
+      <c r="L25" s="140"/>
+      <c r="M25" s="140"/>
+      <c r="N25" s="140"/>
+      <c r="O25" s="140"/>
+      <c r="P25" s="140"/>
+      <c r="Q25" s="140"/>
+      <c r="R25" s="141"/>
     </row>
     <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="63"/>
-      <c r="B26" s="124"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="125"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="125"/>
-      <c r="G26" s="125"/>
-      <c r="H26" s="125"/>
-      <c r="I26" s="125"/>
-      <c r="J26" s="125"/>
-      <c r="K26" s="125"/>
-      <c r="L26" s="125"/>
-      <c r="M26" s="125"/>
-      <c r="N26" s="125"/>
-      <c r="O26" s="125"/>
-      <c r="P26" s="125"/>
-      <c r="Q26" s="125"/>
-      <c r="R26" s="126"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="140"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
+      <c r="K26" s="140"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="140"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="140"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="141"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="63"/>
-      <c r="B27" s="124"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="125"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="125"/>
-      <c r="K27" s="125"/>
-      <c r="L27" s="125"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="125"/>
-      <c r="O27" s="125"/>
-      <c r="P27" s="125"/>
-      <c r="Q27" s="125"/>
-      <c r="R27" s="126"/>
+      <c r="B27" s="139"/>
+      <c r="C27" s="140"/>
+      <c r="D27" s="140"/>
+      <c r="E27" s="140"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="140"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="140"/>
+      <c r="O27" s="140"/>
+      <c r="P27" s="140"/>
+      <c r="Q27" s="140"/>
+      <c r="R27" s="141"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="63"/>
-      <c r="B28" s="124"/>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="125"/>
-      <c r="L28" s="125"/>
-      <c r="M28" s="125"/>
-      <c r="N28" s="125"/>
-      <c r="O28" s="125"/>
-      <c r="P28" s="125"/>
-      <c r="Q28" s="125"/>
-      <c r="R28" s="126"/>
+      <c r="B28" s="139"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="140"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="140"/>
+      <c r="I28" s="140"/>
+      <c r="J28" s="140"/>
+      <c r="K28" s="140"/>
+      <c r="L28" s="140"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="140"/>
+      <c r="O28" s="140"/>
+      <c r="P28" s="140"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="141"/>
     </row>
     <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="63"/>
-      <c r="B29" s="124"/>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
-      <c r="G29" s="125"/>
-      <c r="H29" s="125"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="125"/>
-      <c r="L29" s="125"/>
-      <c r="M29" s="125"/>
-      <c r="N29" s="125"/>
-      <c r="O29" s="125"/>
-      <c r="P29" s="125"/>
-      <c r="Q29" s="125"/>
-      <c r="R29" s="126"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="140"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="140"/>
+      <c r="I29" s="140"/>
+      <c r="J29" s="140"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="140"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="140"/>
+      <c r="O29" s="140"/>
+      <c r="P29" s="140"/>
+      <c r="Q29" s="140"/>
+      <c r="R29" s="141"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="63"/>
-      <c r="B30" s="124"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="125"/>
-      <c r="G30" s="125"/>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="125"/>
-      <c r="L30" s="125"/>
-      <c r="M30" s="125"/>
-      <c r="N30" s="125"/>
-      <c r="O30" s="125"/>
-      <c r="P30" s="125"/>
-      <c r="Q30" s="125"/>
-      <c r="R30" s="126"/>
+      <c r="B30" s="139"/>
+      <c r="C30" s="140"/>
+      <c r="D30" s="140"/>
+      <c r="E30" s="140"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="140"/>
+      <c r="I30" s="140"/>
+      <c r="J30" s="140"/>
+      <c r="K30" s="140"/>
+      <c r="L30" s="140"/>
+      <c r="M30" s="140"/>
+      <c r="N30" s="140"/>
+      <c r="O30" s="140"/>
+      <c r="P30" s="140"/>
+      <c r="Q30" s="140"/>
+      <c r="R30" s="141"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="63"/>
-      <c r="B31" s="124"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="125"/>
-      <c r="H31" s="125"/>
-      <c r="I31" s="125"/>
-      <c r="J31" s="125"/>
-      <c r="K31" s="125"/>
-      <c r="L31" s="125"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="125"/>
-      <c r="O31" s="125"/>
-      <c r="P31" s="125"/>
-      <c r="Q31" s="125"/>
-      <c r="R31" s="126"/>
+      <c r="B31" s="139"/>
+      <c r="C31" s="140"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="140"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="140"/>
+      <c r="H31" s="140"/>
+      <c r="I31" s="140"/>
+      <c r="J31" s="140"/>
+      <c r="K31" s="140"/>
+      <c r="L31" s="140"/>
+      <c r="M31" s="140"/>
+      <c r="N31" s="140"/>
+      <c r="O31" s="140"/>
+      <c r="P31" s="140"/>
+      <c r="Q31" s="140"/>
+      <c r="R31" s="141"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="63"/>
-      <c r="B32" s="124"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="125"/>
-      <c r="E32" s="125"/>
-      <c r="F32" s="125"/>
-      <c r="G32" s="125"/>
-      <c r="H32" s="125"/>
-      <c r="I32" s="125"/>
-      <c r="J32" s="125"/>
-      <c r="K32" s="125"/>
-      <c r="L32" s="125"/>
-      <c r="M32" s="125"/>
-      <c r="N32" s="125"/>
-      <c r="O32" s="125"/>
-      <c r="P32" s="125"/>
-      <c r="Q32" s="125"/>
-      <c r="R32" s="126"/>
+      <c r="B32" s="139"/>
+      <c r="C32" s="140"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="140"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="140"/>
+      <c r="H32" s="140"/>
+      <c r="I32" s="140"/>
+      <c r="J32" s="140"/>
+      <c r="K32" s="140"/>
+      <c r="L32" s="140"/>
+      <c r="M32" s="140"/>
+      <c r="N32" s="140"/>
+      <c r="O32" s="140"/>
+      <c r="P32" s="140"/>
+      <c r="Q32" s="140"/>
+      <c r="R32" s="141"/>
     </row>
     <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="63"/>
-      <c r="B33" s="124"/>
-      <c r="C33" s="125"/>
-      <c r="D33" s="125"/>
-      <c r="E33" s="125"/>
-      <c r="F33" s="125"/>
-      <c r="G33" s="125"/>
-      <c r="H33" s="125"/>
-      <c r="I33" s="125"/>
-      <c r="J33" s="125"/>
-      <c r="K33" s="125"/>
-      <c r="L33" s="125"/>
-      <c r="M33" s="125"/>
-      <c r="N33" s="125"/>
-      <c r="O33" s="125"/>
-      <c r="P33" s="125"/>
-      <c r="Q33" s="125"/>
-      <c r="R33" s="126"/>
+      <c r="B33" s="139"/>
+      <c r="C33" s="140"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="140"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="140"/>
+      <c r="H33" s="140"/>
+      <c r="I33" s="140"/>
+      <c r="J33" s="140"/>
+      <c r="K33" s="140"/>
+      <c r="L33" s="140"/>
+      <c r="M33" s="140"/>
+      <c r="N33" s="140"/>
+      <c r="O33" s="140"/>
+      <c r="P33" s="140"/>
+      <c r="Q33" s="140"/>
+      <c r="R33" s="141"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="63"/>
-      <c r="B34" s="124"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="125"/>
-      <c r="I34" s="125"/>
-      <c r="J34" s="125"/>
-      <c r="K34" s="125"/>
-      <c r="L34" s="125"/>
-      <c r="M34" s="125"/>
-      <c r="N34" s="125"/>
-      <c r="O34" s="125"/>
-      <c r="P34" s="125"/>
-      <c r="Q34" s="125"/>
-      <c r="R34" s="126"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="140"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="140"/>
+      <c r="H34" s="140"/>
+      <c r="I34" s="140"/>
+      <c r="J34" s="140"/>
+      <c r="K34" s="140"/>
+      <c r="L34" s="140"/>
+      <c r="M34" s="140"/>
+      <c r="N34" s="140"/>
+      <c r="O34" s="140"/>
+      <c r="P34" s="140"/>
+      <c r="Q34" s="140"/>
+      <c r="R34" s="141"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="63"/>
-      <c r="B35" s="124"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="125"/>
-      <c r="F35" s="125"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="125"/>
-      <c r="I35" s="125"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="125"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="125"/>
-      <c r="N35" s="125"/>
-      <c r="O35" s="125"/>
-      <c r="P35" s="125"/>
-      <c r="Q35" s="125"/>
-      <c r="R35" s="126"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="140"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="140"/>
+      <c r="H35" s="140"/>
+      <c r="I35" s="140"/>
+      <c r="J35" s="140"/>
+      <c r="K35" s="140"/>
+      <c r="L35" s="140"/>
+      <c r="M35" s="140"/>
+      <c r="N35" s="140"/>
+      <c r="O35" s="140"/>
+      <c r="P35" s="140"/>
+      <c r="Q35" s="140"/>
+      <c r="R35" s="141"/>
     </row>
     <row r="36" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="64"/>
-      <c r="B36" s="115"/>
-      <c r="C36" s="116"/>
-      <c r="D36" s="116"/>
-      <c r="E36" s="116"/>
-      <c r="F36" s="116"/>
-      <c r="G36" s="116"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="116"/>
-      <c r="J36" s="116"/>
-      <c r="K36" s="116"/>
-      <c r="L36" s="116"/>
-      <c r="M36" s="116"/>
-      <c r="N36" s="116"/>
-      <c r="O36" s="116"/>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
-      <c r="R36" s="117"/>
+      <c r="B36" s="153"/>
+      <c r="C36" s="154"/>
+      <c r="D36" s="154"/>
+      <c r="E36" s="154"/>
+      <c r="F36" s="154"/>
+      <c r="G36" s="154"/>
+      <c r="H36" s="154"/>
+      <c r="I36" s="154"/>
+      <c r="J36" s="154"/>
+      <c r="K36" s="154"/>
+      <c r="L36" s="154"/>
+      <c r="M36" s="154"/>
+      <c r="N36" s="154"/>
+      <c r="O36" s="154"/>
+      <c r="P36" s="154"/>
+      <c r="Q36" s="154"/>
+      <c r="R36" s="155"/>
     </row>
     <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="118" t="s">
+      <c r="A37" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="119"/>
-      <c r="E37" s="119"/>
-      <c r="F37" s="119"/>
-      <c r="G37" s="119"/>
-      <c r="H37" s="120"/>
-      <c r="I37" s="118" t="s">
+      <c r="B37" s="157"/>
+      <c r="C37" s="157"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="157"/>
+      <c r="F37" s="157"/>
+      <c r="G37" s="157"/>
+      <c r="H37" s="158"/>
+      <c r="I37" s="156" t="s">
         <v>60</v>
       </c>
-      <c r="J37" s="119"/>
-      <c r="K37" s="119"/>
-      <c r="L37" s="119"/>
-      <c r="M37" s="119"/>
-      <c r="N37" s="119"/>
-      <c r="O37" s="119"/>
-      <c r="P37" s="119"/>
-      <c r="Q37" s="119"/>
-      <c r="R37" s="120"/>
+      <c r="J37" s="157"/>
+      <c r="K37" s="157"/>
+      <c r="L37" s="157"/>
+      <c r="M37" s="157"/>
+      <c r="N37" s="157"/>
+      <c r="O37" s="157"/>
+      <c r="P37" s="157"/>
+      <c r="Q37" s="157"/>
+      <c r="R37" s="158"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="65" t="s">
@@ -6018,22 +6051,22 @@
       <c r="I38" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="J38" s="121" t="s">
+      <c r="J38" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="K38" s="122"/>
+      <c r="K38" s="160"/>
       <c r="L38" s="67" t="s">
         <v>1</v>
       </c>
       <c r="M38" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="N38" s="121" t="s">
+      <c r="N38" s="159" t="s">
         <v>20</v>
       </c>
-      <c r="O38" s="123"/>
-      <c r="P38" s="123"/>
-      <c r="Q38" s="122"/>
+      <c r="O38" s="161"/>
+      <c r="P38" s="161"/>
+      <c r="Q38" s="160"/>
       <c r="R38" s="69" t="s">
         <v>1</v>
       </c>
@@ -6058,18 +6091,18 @@
       <c r="I39" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="J39" s="106" t="s">
+      <c r="J39" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="K39" s="107"/>
+      <c r="K39" s="151"/>
       <c r="L39" s="73" t="s">
         <v>36</v>
       </c>
       <c r="M39" s="74"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="108"/>
-      <c r="P39" s="108"/>
-      <c r="Q39" s="107"/>
+      <c r="N39" s="150"/>
+      <c r="O39" s="152"/>
+      <c r="P39" s="152"/>
+      <c r="Q39" s="151"/>
       <c r="R39" s="76"/>
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6082,14 +6115,14 @@
       <c r="G40" s="72"/>
       <c r="H40" s="75"/>
       <c r="I40" s="70"/>
-      <c r="J40" s="106"/>
-      <c r="K40" s="107"/>
+      <c r="J40" s="150"/>
+      <c r="K40" s="151"/>
       <c r="L40" s="73"/>
       <c r="M40" s="74"/>
-      <c r="N40" s="106"/>
-      <c r="O40" s="108"/>
-      <c r="P40" s="108"/>
-      <c r="Q40" s="107"/>
+      <c r="N40" s="150"/>
+      <c r="O40" s="152"/>
+      <c r="P40" s="152"/>
+      <c r="Q40" s="151"/>
       <c r="R40" s="76"/>
     </row>
     <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6102,14 +6135,14 @@
       <c r="G41" s="72"/>
       <c r="H41" s="75"/>
       <c r="I41" s="70"/>
-      <c r="J41" s="106"/>
-      <c r="K41" s="107"/>
+      <c r="J41" s="150"/>
+      <c r="K41" s="151"/>
       <c r="L41" s="73"/>
       <c r="M41" s="74"/>
-      <c r="N41" s="106"/>
-      <c r="O41" s="108"/>
-      <c r="P41" s="108"/>
-      <c r="Q41" s="107"/>
+      <c r="N41" s="150"/>
+      <c r="O41" s="152"/>
+      <c r="P41" s="152"/>
+      <c r="Q41" s="151"/>
       <c r="R41" s="76"/>
     </row>
     <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6122,14 +6155,14 @@
       <c r="G42" s="72"/>
       <c r="H42" s="75"/>
       <c r="I42" s="70"/>
-      <c r="J42" s="106"/>
-      <c r="K42" s="107"/>
+      <c r="J42" s="150"/>
+      <c r="K42" s="151"/>
       <c r="L42" s="73"/>
       <c r="M42" s="74"/>
-      <c r="N42" s="106"/>
-      <c r="O42" s="108"/>
-      <c r="P42" s="108"/>
-      <c r="Q42" s="107"/>
+      <c r="N42" s="150"/>
+      <c r="O42" s="152"/>
+      <c r="P42" s="152"/>
+      <c r="Q42" s="151"/>
       <c r="R42" s="76"/>
     </row>
     <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6142,14 +6175,14 @@
       <c r="G43" s="72"/>
       <c r="H43" s="75"/>
       <c r="I43" s="70"/>
-      <c r="J43" s="106"/>
-      <c r="K43" s="107"/>
+      <c r="J43" s="150"/>
+      <c r="K43" s="151"/>
       <c r="L43" s="73"/>
       <c r="M43" s="74"/>
-      <c r="N43" s="106"/>
-      <c r="O43" s="108"/>
-      <c r="P43" s="108"/>
-      <c r="Q43" s="107"/>
+      <c r="N43" s="150"/>
+      <c r="O43" s="152"/>
+      <c r="P43" s="152"/>
+      <c r="Q43" s="151"/>
       <c r="R43" s="76"/>
     </row>
     <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6162,14 +6195,14 @@
       <c r="G44" s="72"/>
       <c r="H44" s="75"/>
       <c r="I44" s="70"/>
-      <c r="J44" s="106"/>
-      <c r="K44" s="107"/>
+      <c r="J44" s="150"/>
+      <c r="K44" s="151"/>
       <c r="L44" s="73"/>
       <c r="M44" s="74"/>
-      <c r="N44" s="106"/>
-      <c r="O44" s="108"/>
-      <c r="P44" s="108"/>
-      <c r="Q44" s="107"/>
+      <c r="N44" s="150"/>
+      <c r="O44" s="152"/>
+      <c r="P44" s="152"/>
+      <c r="Q44" s="151"/>
       <c r="R44" s="76"/>
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6182,14 +6215,14 @@
       <c r="G45" s="72"/>
       <c r="H45" s="75"/>
       <c r="I45" s="70"/>
-      <c r="J45" s="106"/>
-      <c r="K45" s="107"/>
+      <c r="J45" s="150"/>
+      <c r="K45" s="151"/>
       <c r="L45" s="73"/>
       <c r="M45" s="74"/>
-      <c r="N45" s="106"/>
-      <c r="O45" s="108"/>
-      <c r="P45" s="108"/>
-      <c r="Q45" s="107"/>
+      <c r="N45" s="150"/>
+      <c r="O45" s="152"/>
+      <c r="P45" s="152"/>
+      <c r="Q45" s="151"/>
       <c r="R45" s="76"/>
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6202,14 +6235,14 @@
       <c r="G46" s="72"/>
       <c r="H46" s="75"/>
       <c r="I46" s="70"/>
-      <c r="J46" s="106"/>
-      <c r="K46" s="107"/>
+      <c r="J46" s="150"/>
+      <c r="K46" s="151"/>
       <c r="L46" s="73"/>
       <c r="M46" s="74"/>
-      <c r="N46" s="106"/>
-      <c r="O46" s="108"/>
-      <c r="P46" s="108"/>
-      <c r="Q46" s="107"/>
+      <c r="N46" s="150"/>
+      <c r="O46" s="152"/>
+      <c r="P46" s="152"/>
+      <c r="Q46" s="151"/>
       <c r="R46" s="76"/>
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6222,14 +6255,14 @@
       <c r="G47" s="72"/>
       <c r="H47" s="75"/>
       <c r="I47" s="70"/>
-      <c r="J47" s="106"/>
-      <c r="K47" s="107"/>
+      <c r="J47" s="150"/>
+      <c r="K47" s="151"/>
       <c r="L47" s="73"/>
       <c r="M47" s="74"/>
-      <c r="N47" s="106"/>
-      <c r="O47" s="108"/>
-      <c r="P47" s="108"/>
-      <c r="Q47" s="107"/>
+      <c r="N47" s="150"/>
+      <c r="O47" s="152"/>
+      <c r="P47" s="152"/>
+      <c r="Q47" s="151"/>
       <c r="R47" s="76"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6242,14 +6275,14 @@
       <c r="G48" s="72"/>
       <c r="H48" s="75"/>
       <c r="I48" s="70"/>
-      <c r="J48" s="106"/>
-      <c r="K48" s="107"/>
+      <c r="J48" s="150"/>
+      <c r="K48" s="151"/>
       <c r="L48" s="73"/>
       <c r="M48" s="74"/>
-      <c r="N48" s="106"/>
-      <c r="O48" s="108"/>
-      <c r="P48" s="108"/>
-      <c r="Q48" s="107"/>
+      <c r="N48" s="150"/>
+      <c r="O48" s="152"/>
+      <c r="P48" s="152"/>
+      <c r="Q48" s="151"/>
       <c r="R48" s="76"/>
     </row>
     <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6262,14 +6295,14 @@
       <c r="G49" s="72"/>
       <c r="H49" s="75"/>
       <c r="I49" s="70"/>
-      <c r="J49" s="106"/>
-      <c r="K49" s="107"/>
+      <c r="J49" s="150"/>
+      <c r="K49" s="151"/>
       <c r="L49" s="73"/>
       <c r="M49" s="74"/>
-      <c r="N49" s="106"/>
-      <c r="O49" s="108"/>
-      <c r="P49" s="108"/>
-      <c r="Q49" s="107"/>
+      <c r="N49" s="150"/>
+      <c r="O49" s="152"/>
+      <c r="P49" s="152"/>
+      <c r="Q49" s="151"/>
       <c r="R49" s="76"/>
     </row>
     <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6282,14 +6315,14 @@
       <c r="G50" s="72"/>
       <c r="H50" s="75"/>
       <c r="I50" s="70"/>
-      <c r="J50" s="106"/>
-      <c r="K50" s="107"/>
+      <c r="J50" s="150"/>
+      <c r="K50" s="151"/>
       <c r="L50" s="73"/>
       <c r="M50" s="74"/>
-      <c r="N50" s="106"/>
-      <c r="O50" s="108"/>
-      <c r="P50" s="108"/>
-      <c r="Q50" s="107"/>
+      <c r="N50" s="150"/>
+      <c r="O50" s="152"/>
+      <c r="P50" s="152"/>
+      <c r="Q50" s="151"/>
       <c r="R50" s="76"/>
     </row>
     <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6302,14 +6335,14 @@
       <c r="G51" s="72"/>
       <c r="H51" s="75"/>
       <c r="I51" s="70"/>
-      <c r="J51" s="106"/>
-      <c r="K51" s="107"/>
+      <c r="J51" s="150"/>
+      <c r="K51" s="151"/>
       <c r="L51" s="73"/>
       <c r="M51" s="74"/>
-      <c r="N51" s="106"/>
-      <c r="O51" s="108"/>
-      <c r="P51" s="108"/>
-      <c r="Q51" s="107"/>
+      <c r="N51" s="150"/>
+      <c r="O51" s="152"/>
+      <c r="P51" s="152"/>
+      <c r="Q51" s="151"/>
       <c r="R51" s="76"/>
     </row>
     <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -6322,14 +6355,14 @@
       <c r="G52" s="72"/>
       <c r="H52" s="75"/>
       <c r="I52" s="70"/>
-      <c r="J52" s="106"/>
-      <c r="K52" s="107"/>
+      <c r="J52" s="150"/>
+      <c r="K52" s="151"/>
       <c r="L52" s="73"/>
       <c r="M52" s="74"/>
-      <c r="N52" s="106"/>
-      <c r="O52" s="108"/>
-      <c r="P52" s="108"/>
-      <c r="Q52" s="107"/>
+      <c r="N52" s="150"/>
+      <c r="O52" s="152"/>
+      <c r="P52" s="152"/>
+      <c r="Q52" s="151"/>
       <c r="R52" s="76"/>
     </row>
     <row r="53" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6342,44 +6375,136 @@
       <c r="G53" s="79"/>
       <c r="H53" s="82"/>
       <c r="I53" s="77"/>
-      <c r="J53" s="106"/>
-      <c r="K53" s="107"/>
+      <c r="J53" s="150"/>
+      <c r="K53" s="151"/>
       <c r="L53" s="80"/>
       <c r="M53" s="81"/>
-      <c r="N53" s="106"/>
-      <c r="O53" s="108"/>
-      <c r="P53" s="108"/>
-      <c r="Q53" s="107"/>
+      <c r="N53" s="150"/>
+      <c r="O53" s="152"/>
+      <c r="P53" s="152"/>
+      <c r="Q53" s="151"/>
       <c r="R53" s="76"/>
     </row>
     <row r="54" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="109" t="s">
+      <c r="A54" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="110"/>
-      <c r="C54" s="111">
+      <c r="B54" s="163"/>
+      <c r="C54" s="164">
         <v>0</v>
       </c>
-      <c r="D54" s="112"/>
-      <c r="E54" s="113" t="s">
+      <c r="D54" s="165"/>
+      <c r="E54" s="166" t="s">
         <v>66</v>
       </c>
-      <c r="F54" s="114"/>
-      <c r="G54" s="114"/>
-      <c r="H54" s="114"/>
-      <c r="I54" s="114"/>
-      <c r="J54" s="114"/>
-      <c r="K54" s="114"/>
-      <c r="L54" s="114"/>
-      <c r="M54" s="114"/>
-      <c r="N54" s="114"/>
-      <c r="O54" s="114"/>
-      <c r="P54" s="114"/>
-      <c r="Q54" s="114"/>
-      <c r="R54" s="114"/>
+      <c r="F54" s="167"/>
+      <c r="G54" s="167"/>
+      <c r="H54" s="167"/>
+      <c r="I54" s="167"/>
+      <c r="J54" s="167"/>
+      <c r="K54" s="167"/>
+      <c r="L54" s="167"/>
+      <c r="M54" s="167"/>
+      <c r="N54" s="167"/>
+      <c r="O54" s="167"/>
+      <c r="P54" s="167"/>
+      <c r="Q54" s="167"/>
+      <c r="R54" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="N52:Q52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="N53:Q53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:R54"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="N49:Q49"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="N50:Q50"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="N51:Q51"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="N46:Q46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="N47:Q47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="N48:Q48"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="N45:Q45"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="N41:Q41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="B36:R36"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="I37:R37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="B30:R30"/>
+    <mergeCell ref="B31:R31"/>
+    <mergeCell ref="B33:R33"/>
+    <mergeCell ref="B34:R34"/>
+    <mergeCell ref="B35:R35"/>
+    <mergeCell ref="B32:R32"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B24:R24"/>
+    <mergeCell ref="B25:R25"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="B27:R27"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B17:R17"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B19:R19"/>
+    <mergeCell ref="B20:R20"/>
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:R13"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B15:R15"/>
+    <mergeCell ref="B16:R16"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:R10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:R11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="K12:R12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -6396,98 +6521,6 @@
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:R2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:R8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:L5"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="D7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:R10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:R11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="K12:R12"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:R9"/>
-    <mergeCell ref="B17:R17"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B19:R19"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:R13"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B15:R15"/>
-    <mergeCell ref="B16:R16"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="B30:R30"/>
-    <mergeCell ref="B31:R31"/>
-    <mergeCell ref="B33:R33"/>
-    <mergeCell ref="B34:R34"/>
-    <mergeCell ref="B35:R35"/>
-    <mergeCell ref="B32:R32"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B24:R24"/>
-    <mergeCell ref="B25:R25"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="B27:R27"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="N41:Q41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="B36:R36"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="I37:R37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="N39:Q39"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="N46:Q46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="N47:Q47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="N48:Q48"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="N44:Q44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="N45:Q45"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="N52:Q52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="N53:Q53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:R54"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="N49:Q49"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="N50:Q50"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="N51:Q51"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Input" error="Please select a valid options in the dropdown list." sqref="Q5">
@@ -6506,8 +6539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AM41"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6520,75 +6553,75 @@
   <sheetData>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="174" t="s">
+      <c r="A3" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="170" t="s">
+      <c r="B3" s="168" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="174" t="s">
+      <c r="C3" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="174" t="s">
+      <c r="D3" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="179"/>
-      <c r="G3" s="167" t="s">
+      <c r="F3" s="175"/>
+      <c r="G3" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="168"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="167" t="s">
+      <c r="H3" s="179"/>
+      <c r="I3" s="180"/>
+      <c r="J3" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="168"/>
-      <c r="L3" s="169"/>
-      <c r="M3" s="167" t="s">
+      <c r="K3" s="179"/>
+      <c r="L3" s="180"/>
+      <c r="M3" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="169"/>
+      <c r="N3" s="180"/>
       <c r="O3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="167" t="s">
+      <c r="Q3" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="168"/>
-      <c r="S3" s="169"/>
-      <c r="T3" s="167" t="s">
+      <c r="R3" s="179"/>
+      <c r="S3" s="180"/>
+      <c r="T3" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="168"/>
-      <c r="V3" s="169"/>
-      <c r="W3" s="167" t="s">
+      <c r="U3" s="179"/>
+      <c r="V3" s="180"/>
+      <c r="W3" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="X3" s="168"/>
-      <c r="Y3" s="169"/>
-      <c r="Z3" s="170" t="s">
+      <c r="X3" s="179"/>
+      <c r="Y3" s="180"/>
+      <c r="Z3" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="AA3" s="170" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB3" s="174" t="s">
+      <c r="AA3" s="168" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB3" s="172" t="s">
         <v>25</v>
       </c>
-      <c r="AC3" s="172" t="s">
+      <c r="AC3" s="181" t="s">
         <v>26</v>
       </c>
-      <c r="AD3" s="173"/>
-      <c r="AE3" s="170" t="s">
+      <c r="AD3" s="182"/>
+      <c r="AE3" s="168" t="s">
         <v>67</v>
       </c>
-      <c r="AF3" s="170" t="s">
-        <v>86</v>
+      <c r="AF3" s="168" t="s">
+        <v>84</v>
       </c>
       <c r="AG3" s="97"/>
       <c r="AH3" s="97"/>
@@ -6599,26 +6632,26 @@
       <c r="AM3" s="97"/>
     </row>
     <row r="4" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="175"/>
-      <c r="B4" s="175"/>
-      <c r="C4" s="175"/>
-      <c r="D4" s="175"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="181"/>
+      <c r="A4" s="173"/>
+      <c r="B4" s="173"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="173"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="177"/>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="176" t="s">
+      <c r="H4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="177"/>
+      <c r="I4" s="171"/>
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="176" t="s">
+      <c r="K4" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="177"/>
+      <c r="L4" s="171"/>
       <c r="M4" s="2" t="s">
         <v>16</v>
       </c>
@@ -6643,28 +6676,28 @@
       <c r="T4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U4" s="176" t="s">
+      <c r="U4" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="177"/>
+      <c r="V4" s="171"/>
       <c r="W4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="176" t="s">
+      <c r="X4" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="177"/>
-      <c r="Z4" s="171"/>
-      <c r="AA4" s="171"/>
-      <c r="AB4" s="175"/>
+      <c r="Y4" s="171"/>
+      <c r="Z4" s="169"/>
+      <c r="AA4" s="169"/>
+      <c r="AB4" s="173"/>
       <c r="AC4" s="48" t="s">
         <v>27</v>
       </c>
       <c r="AD4" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="175"/>
-      <c r="AF4" s="171"/>
+      <c r="AE4" s="173"/>
+      <c r="AF4" s="169"/>
       <c r="AG4" s="97"/>
       <c r="AH4" s="97"/>
       <c r="AI4" s="97"/>
@@ -6892,7 +6925,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
@@ -7004,8 +7037,12 @@
       <c r="AF10" s="29"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>87</v>
+      </c>
       <c r="C11" s="19"/>
       <c r="D11" s="18"/>
       <c r="E11" s="31"/>
@@ -7047,9 +7084,7 @@
       <c r="AM11" s="97"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>81</v>
-      </c>
+      <c r="A12" s="18"/>
       <c r="B12" s="25"/>
       <c r="C12" s="19"/>
       <c r="D12" s="18"/>
@@ -7092,15 +7127,31 @@
       <c r="AM12" s="97"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="B13" s="25"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="22"/>
+      <c r="C13" s="19">
+        <v>1</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="31">
+        <v>30</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0</v>
+      </c>
+      <c r="G13" s="20">
+        <v>2</v>
+      </c>
+      <c r="H13" s="21">
+        <v>2</v>
+      </c>
+      <c r="I13" s="22">
+        <v>0</v>
+      </c>
       <c r="J13" s="20"/>
       <c r="K13" s="21"/>
       <c r="L13" s="22"/>
@@ -7221,15 +7272,33 @@
       <c r="AM15" s="97"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
+      <c r="A16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="31">
+        <v>30</v>
+      </c>
+      <c r="F16" s="22">
+        <v>0</v>
+      </c>
+      <c r="G16" s="20">
+        <v>2</v>
+      </c>
+      <c r="H16" s="21">
+        <v>2</v>
+      </c>
+      <c r="I16" s="22">
+        <v>0</v>
+      </c>
       <c r="J16" s="20"/>
       <c r="K16" s="21"/>
       <c r="L16" s="22"/>
@@ -7307,9 +7376,7 @@
       <c r="AM17" s="97"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>82</v>
-      </c>
+      <c r="A18" s="18"/>
       <c r="B18" s="25"/>
       <c r="C18" s="19"/>
       <c r="D18" s="18"/>
@@ -7395,15 +7462,33 @@
       <c r="AM19" s="97"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
+      <c r="A20" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="31">
+        <v>30</v>
+      </c>
+      <c r="F20" s="22">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="21">
+        <v>2</v>
+      </c>
+      <c r="I20" s="22">
+        <v>0</v>
+      </c>
       <c r="J20" s="20"/>
       <c r="K20" s="21"/>
       <c r="L20" s="22"/>
@@ -7567,15 +7652,33 @@
       <c r="AM23" s="97"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="22"/>
+      <c r="A24" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="31">
+        <v>30</v>
+      </c>
+      <c r="F24" s="22">
+        <v>0</v>
+      </c>
+      <c r="G24" s="20">
+        <v>2</v>
+      </c>
+      <c r="H24" s="21">
+        <v>2</v>
+      </c>
+      <c r="I24" s="22">
+        <v>0</v>
+      </c>
       <c r="J24" s="20"/>
       <c r="K24" s="21"/>
       <c r="L24" s="22"/>
@@ -7610,9 +7713,7 @@
       <c r="AM24" s="97"/>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="A25" s="18"/>
       <c r="B25" s="25"/>
       <c r="C25" s="19"/>
       <c r="D25" s="18"/>
@@ -7655,15 +7756,33 @@
       <c r="AM25" s="97"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="22"/>
+      <c r="A26" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="31">
+        <v>30</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0</v>
+      </c>
+      <c r="G26" s="20">
+        <v>2</v>
+      </c>
+      <c r="H26" s="21">
+        <v>2</v>
+      </c>
+      <c r="I26" s="22">
+        <v>0</v>
+      </c>
       <c r="J26" s="20"/>
       <c r="K26" s="21"/>
       <c r="L26" s="22"/>
@@ -7827,15 +7946,33 @@
       <c r="AM29" s="97"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="22"/>
+      <c r="A30" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="31">
+        <v>30</v>
+      </c>
+      <c r="F30" s="22">
+        <v>0</v>
+      </c>
+      <c r="G30" s="20">
+        <v>2</v>
+      </c>
+      <c r="H30" s="21">
+        <v>2</v>
+      </c>
+      <c r="I30" s="22">
+        <v>0</v>
+      </c>
       <c r="J30" s="20"/>
       <c r="K30" s="21"/>
       <c r="L30" s="22"/>
@@ -7913,15 +8050,33 @@
       <c r="AM31" s="97"/>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="22"/>
+      <c r="A32" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="19">
+        <v>1</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="31">
+        <v>30</v>
+      </c>
+      <c r="F32" s="22">
+        <v>0</v>
+      </c>
+      <c r="G32" s="20">
+        <v>2</v>
+      </c>
+      <c r="H32" s="21">
+        <v>2</v>
+      </c>
+      <c r="I32" s="22">
+        <v>0</v>
+      </c>
       <c r="J32" s="20"/>
       <c r="K32" s="21"/>
       <c r="L32" s="22"/>
@@ -7956,9 +8111,7 @@
       <c r="AM32" s="97"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>84</v>
-      </c>
+      <c r="A33" s="18"/>
       <c r="B33" s="25"/>
       <c r="C33" s="19"/>
       <c r="D33" s="18"/>
@@ -8087,15 +8240,33 @@
       <c r="AM35" s="97"/>
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="22"/>
+      <c r="A36" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="19">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="31">
+        <v>30</v>
+      </c>
+      <c r="F36" s="22">
+        <v>0</v>
+      </c>
+      <c r="G36" s="20">
+        <v>2</v>
+      </c>
+      <c r="H36" s="21">
+        <v>2</v>
+      </c>
+      <c r="I36" s="22">
+        <v>0</v>
+      </c>
       <c r="J36" s="20"/>
       <c r="K36" s="21"/>
       <c r="L36" s="22"/>
@@ -8216,15 +8387,33 @@
       <c r="AM38" s="97"/>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="22"/>
+      <c r="A39" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="31">
+        <v>30</v>
+      </c>
+      <c r="F39" s="22">
+        <v>0</v>
+      </c>
+      <c r="G39" s="20">
+        <v>2</v>
+      </c>
+      <c r="H39" s="21">
+        <v>2</v>
+      </c>
+      <c r="I39" s="22">
+        <v>0</v>
+      </c>
       <c r="J39" s="20"/>
       <c r="K39" s="21"/>
       <c r="L39" s="22"/>
@@ -8346,6 +8535,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AA3:AA4"/>
     <mergeCell ref="AF3:AF4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="X4:Y4"/>
@@ -8362,11 +8556,6 @@
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="T3:V3"/>
     <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AA3:AA4"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bad Input" error="Input for this cell must be one of the listed positions and all uppercase!" sqref="S5:S41">
@@ -8394,8 +8583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8497,93 +8686,93 @@
       </c>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="179"/>
-      <c r="E2" s="167" t="s">
+      <c r="D2" s="175"/>
+      <c r="E2" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="167" t="s">
+      <c r="F2" s="179"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="167" t="s">
+      <c r="I2" s="179"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="169"/>
+      <c r="L2" s="180"/>
       <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="167" t="s">
+      <c r="O2" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="169"/>
-      <c r="R2" s="167" t="s">
+      <c r="P2" s="179"/>
+      <c r="Q2" s="180"/>
+      <c r="R2" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="168"/>
-      <c r="T2" s="169"/>
-      <c r="U2" s="167" t="s">
+      <c r="S2" s="179"/>
+      <c r="T2" s="180"/>
+      <c r="U2" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="168"/>
-      <c r="W2" s="169"/>
-      <c r="X2" s="170" t="s">
+      <c r="V2" s="179"/>
+      <c r="W2" s="180"/>
+      <c r="X2" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="170" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z2" s="174" t="s">
+      <c r="Y2" s="168" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z2" s="172" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="172" t="s">
+      <c r="AA2" s="181" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="173"/>
-      <c r="AC2" s="170" t="s">
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="168" t="s">
         <v>67</v>
       </c>
-      <c r="AD2" s="172" t="s">
+      <c r="AD2" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="AE2" s="191"/>
-      <c r="AF2" s="191"/>
-      <c r="AG2" s="173"/>
+      <c r="AE2" s="189"/>
+      <c r="AF2" s="189"/>
+      <c r="AG2" s="182"/>
     </row>
     <row r="3" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="175"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="180"/>
-      <c r="D3" s="181"/>
+      <c r="A3" s="173"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="177"/>
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="177"/>
+      <c r="G3" s="171"/>
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="176" t="s">
+      <c r="I3" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="177"/>
+      <c r="J3" s="171"/>
       <c r="K3" s="2" t="s">
         <v>16</v>
       </c>
@@ -8608,31 +8797,31 @@
       <c r="R3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="176" t="s">
+      <c r="S3" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="177"/>
+      <c r="T3" s="171"/>
       <c r="U3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="176" t="s">
+      <c r="V3" s="170" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="177"/>
-      <c r="X3" s="171"/>
-      <c r="Y3" s="171"/>
-      <c r="Z3" s="175"/>
+      <c r="W3" s="171"/>
+      <c r="X3" s="169"/>
+      <c r="Y3" s="169"/>
+      <c r="Z3" s="173"/>
       <c r="AA3" s="48" t="s">
         <v>27</v>
       </c>
       <c r="AB3" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" s="175"/>
-      <c r="AD3" s="192"/>
-      <c r="AE3" s="193"/>
-      <c r="AF3" s="193"/>
-      <c r="AG3" s="194"/>
+      <c r="AC3" s="173"/>
+      <c r="AD3" s="190"/>
+      <c r="AE3" s="191"/>
+      <c r="AF3" s="191"/>
+      <c r="AG3" s="192"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
@@ -8659,17 +8848,17 @@
       <c r="V4" s="15"/>
       <c r="W4" s="16"/>
       <c r="X4" s="17"/>
-      <c r="Y4" s="195"/>
+      <c r="Y4" s="106"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
       <c r="AB4" s="12"/>
       <c r="AC4" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" s="188"/>
-      <c r="AE4" s="189"/>
-      <c r="AF4" s="189"/>
-      <c r="AG4" s="190"/>
+      <c r="AD4" s="186"/>
+      <c r="AE4" s="187"/>
+      <c r="AF4" s="187"/>
+      <c r="AG4" s="188"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -8698,7 +8887,7 @@
         <v>76</v>
       </c>
       <c r="R5" s="28">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="S5" s="21"/>
       <c r="T5" s="22"/>
@@ -8711,10 +8900,10 @@
       <c r="AA5" s="25"/>
       <c r="AB5" s="26"/>
       <c r="AC5" s="25"/>
-      <c r="AD5" s="185"/>
-      <c r="AE5" s="186"/>
-      <c r="AF5" s="186"/>
-      <c r="AG5" s="187"/>
+      <c r="AD5" s="183"/>
+      <c r="AE5" s="184"/>
+      <c r="AF5" s="184"/>
+      <c r="AG5" s="185"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
@@ -8746,14 +8935,14 @@
       <c r="AA6" s="25"/>
       <c r="AB6" s="26"/>
       <c r="AC6" s="25"/>
-      <c r="AD6" s="185"/>
-      <c r="AE6" s="186"/>
-      <c r="AF6" s="186"/>
-      <c r="AG6" s="187"/>
+      <c r="AD6" s="183"/>
+      <c r="AE6" s="184"/>
+      <c r="AF6" s="184"/>
+      <c r="AG6" s="185"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="31"/>
@@ -8772,13 +8961,13 @@
         <v>74</v>
       </c>
       <c r="P7" s="27" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="Q7" s="43" t="s">
         <v>76</v>
       </c>
       <c r="R7" s="28">
-        <v>500</v>
+        <v>930</v>
       </c>
       <c r="S7" s="21"/>
       <c r="T7" s="22"/>
@@ -8791,10 +8980,10 @@
       <c r="AA7" s="25"/>
       <c r="AB7" s="26"/>
       <c r="AC7" s="25"/>
-      <c r="AD7" s="185"/>
-      <c r="AE7" s="186"/>
-      <c r="AF7" s="186"/>
-      <c r="AG7" s="187"/>
+      <c r="AD7" s="183"/>
+      <c r="AE7" s="184"/>
+      <c r="AF7" s="184"/>
+      <c r="AG7" s="185"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
@@ -8811,10 +9000,18 @@
       <c r="L8" s="24"/>
       <c r="M8" s="25"/>
       <c r="N8" s="25"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="43"/>
-      <c r="R8" s="28"/>
+      <c r="O8" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q8" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8" s="28">
+        <v>20</v>
+      </c>
       <c r="S8" s="21"/>
       <c r="T8" s="22"/>
       <c r="U8" s="28"/>
@@ -8826,10 +9023,10 @@
       <c r="AA8" s="25"/>
       <c r="AB8" s="26"/>
       <c r="AC8" s="25"/>
-      <c r="AD8" s="185"/>
-      <c r="AE8" s="186"/>
-      <c r="AF8" s="186"/>
-      <c r="AG8" s="187"/>
+      <c r="AD8" s="183"/>
+      <c r="AE8" s="184"/>
+      <c r="AF8" s="184"/>
+      <c r="AG8" s="185"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
@@ -8861,10 +9058,10 @@
       <c r="AA9" s="25"/>
       <c r="AB9" s="26"/>
       <c r="AC9" s="25"/>
-      <c r="AD9" s="185"/>
-      <c r="AE9" s="186"/>
-      <c r="AF9" s="186"/>
-      <c r="AG9" s="187"/>
+      <c r="AD9" s="183"/>
+      <c r="AE9" s="184"/>
+      <c r="AF9" s="184"/>
+      <c r="AG9" s="185"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
@@ -8896,16 +9093,24 @@
       <c r="AA10" s="25"/>
       <c r="AB10" s="26"/>
       <c r="AC10" s="25"/>
-      <c r="AD10" s="185"/>
-      <c r="AE10" s="186"/>
-      <c r="AF10" s="186"/>
-      <c r="AG10" s="187"/>
+      <c r="AD10" s="183"/>
+      <c r="AE10" s="184"/>
+      <c r="AF10" s="184"/>
+      <c r="AG10" s="185"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="31">
+        <v>40</v>
+      </c>
+      <c r="D11" s="22">
+        <v>0</v>
+      </c>
       <c r="E11" s="20"/>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -8931,10 +9136,10 @@
       <c r="AA11" s="25"/>
       <c r="AB11" s="26"/>
       <c r="AC11" s="25"/>
-      <c r="AD11" s="185"/>
-      <c r="AE11" s="186"/>
-      <c r="AF11" s="186"/>
-      <c r="AG11" s="187"/>
+      <c r="AD11" s="183"/>
+      <c r="AE11" s="184"/>
+      <c r="AF11" s="184"/>
+      <c r="AG11" s="185"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
@@ -8966,10 +9171,10 @@
       <c r="AA12" s="25"/>
       <c r="AB12" s="26"/>
       <c r="AC12" s="25"/>
-      <c r="AD12" s="185"/>
-      <c r="AE12" s="186"/>
-      <c r="AF12" s="186"/>
-      <c r="AG12" s="187"/>
+      <c r="AD12" s="183"/>
+      <c r="AE12" s="184"/>
+      <c r="AF12" s="184"/>
+      <c r="AG12" s="185"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
@@ -9001,13 +9206,15 @@
       <c r="AA13" s="25"/>
       <c r="AB13" s="26"/>
       <c r="AC13" s="25"/>
-      <c r="AD13" s="185"/>
-      <c r="AE13" s="186"/>
-      <c r="AF13" s="186"/>
-      <c r="AG13" s="187"/>
+      <c r="AD13" s="183"/>
+      <c r="AE13" s="184"/>
+      <c r="AF13" s="184"/>
+      <c r="AG13" s="185"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="B14" s="18"/>
       <c r="C14" s="31"/>
       <c r="D14" s="22"/>
@@ -9021,10 +9228,18 @@
       <c r="L14" s="24"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="28"/>
+      <c r="O14" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q14" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="R14" s="28">
+        <v>20</v>
+      </c>
       <c r="S14" s="21"/>
       <c r="T14" s="22"/>
       <c r="U14" s="28"/>
@@ -9036,10 +9251,10 @@
       <c r="AA14" s="25"/>
       <c r="AB14" s="26"/>
       <c r="AC14" s="25"/>
-      <c r="AD14" s="185"/>
-      <c r="AE14" s="186"/>
-      <c r="AF14" s="186"/>
-      <c r="AG14" s="187"/>
+      <c r="AD14" s="183"/>
+      <c r="AE14" s="184"/>
+      <c r="AF14" s="184"/>
+      <c r="AG14" s="185"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
@@ -9071,10 +9286,10 @@
       <c r="AA15" s="25"/>
       <c r="AB15" s="26"/>
       <c r="AC15" s="25"/>
-      <c r="AD15" s="185"/>
-      <c r="AE15" s="186"/>
-      <c r="AF15" s="186"/>
-      <c r="AG15" s="187"/>
+      <c r="AD15" s="183"/>
+      <c r="AE15" s="184"/>
+      <c r="AF15" s="184"/>
+      <c r="AG15" s="185"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -9106,10 +9321,10 @@
       <c r="AA16" s="25"/>
       <c r="AB16" s="26"/>
       <c r="AC16" s="25"/>
-      <c r="AD16" s="185"/>
-      <c r="AE16" s="186"/>
-      <c r="AF16" s="186"/>
-      <c r="AG16" s="187"/>
+      <c r="AD16" s="183"/>
+      <c r="AE16" s="184"/>
+      <c r="AF16" s="184"/>
+      <c r="AG16" s="185"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
@@ -9141,10 +9356,10 @@
       <c r="AA17" s="25"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="25"/>
-      <c r="AD17" s="185"/>
-      <c r="AE17" s="186"/>
-      <c r="AF17" s="186"/>
-      <c r="AG17" s="187"/>
+      <c r="AD17" s="183"/>
+      <c r="AE17" s="184"/>
+      <c r="AF17" s="184"/>
+      <c r="AG17" s="185"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
@@ -9176,10 +9391,10 @@
       <c r="AA18" s="25"/>
       <c r="AB18" s="26"/>
       <c r="AC18" s="25"/>
-      <c r="AD18" s="185"/>
-      <c r="AE18" s="186"/>
-      <c r="AF18" s="186"/>
-      <c r="AG18" s="187"/>
+      <c r="AD18" s="183"/>
+      <c r="AE18" s="184"/>
+      <c r="AF18" s="184"/>
+      <c r="AG18" s="185"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -9211,10 +9426,10 @@
       <c r="AA19" s="25"/>
       <c r="AB19" s="26"/>
       <c r="AC19" s="25"/>
-      <c r="AD19" s="185"/>
-      <c r="AE19" s="186"/>
-      <c r="AF19" s="186"/>
-      <c r="AG19" s="187"/>
+      <c r="AD19" s="183"/>
+      <c r="AE19" s="184"/>
+      <c r="AF19" s="184"/>
+      <c r="AG19" s="185"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -9246,10 +9461,10 @@
       <c r="AA20" s="25"/>
       <c r="AB20" s="26"/>
       <c r="AC20" s="25"/>
-      <c r="AD20" s="185"/>
-      <c r="AE20" s="186"/>
-      <c r="AF20" s="186"/>
-      <c r="AG20" s="187"/>
+      <c r="AD20" s="183"/>
+      <c r="AE20" s="184"/>
+      <c r="AF20" s="184"/>
+      <c r="AG20" s="185"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
@@ -9281,10 +9496,10 @@
       <c r="AA21" s="25"/>
       <c r="AB21" s="26"/>
       <c r="AC21" s="25"/>
-      <c r="AD21" s="185"/>
-      <c r="AE21" s="186"/>
-      <c r="AF21" s="186"/>
-      <c r="AG21" s="187"/>
+      <c r="AD21" s="183"/>
+      <c r="AE21" s="184"/>
+      <c r="AF21" s="184"/>
+      <c r="AG21" s="185"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
@@ -9316,10 +9531,10 @@
       <c r="AA22" s="25"/>
       <c r="AB22" s="26"/>
       <c r="AC22" s="25"/>
-      <c r="AD22" s="185"/>
-      <c r="AE22" s="186"/>
-      <c r="AF22" s="186"/>
-      <c r="AG22" s="187"/>
+      <c r="AD22" s="183"/>
+      <c r="AE22" s="184"/>
+      <c r="AF22" s="184"/>
+      <c r="AG22" s="185"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
@@ -9351,10 +9566,10 @@
       <c r="AA23" s="25"/>
       <c r="AB23" s="26"/>
       <c r="AC23" s="25"/>
-      <c r="AD23" s="185"/>
-      <c r="AE23" s="186"/>
-      <c r="AF23" s="186"/>
-      <c r="AG23" s="187"/>
+      <c r="AD23" s="183"/>
+      <c r="AE23" s="184"/>
+      <c r="AF23" s="184"/>
+      <c r="AG23" s="185"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
@@ -9386,10 +9601,10 @@
       <c r="AA24" s="25"/>
       <c r="AB24" s="26"/>
       <c r="AC24" s="25"/>
-      <c r="AD24" s="185"/>
-      <c r="AE24" s="186"/>
-      <c r="AF24" s="186"/>
-      <c r="AG24" s="187"/>
+      <c r="AD24" s="183"/>
+      <c r="AE24" s="184"/>
+      <c r="AF24" s="184"/>
+      <c r="AG24" s="185"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
@@ -9421,10 +9636,10 @@
       <c r="AA25" s="25"/>
       <c r="AB25" s="26"/>
       <c r="AC25" s="25"/>
-      <c r="AD25" s="185"/>
-      <c r="AE25" s="186"/>
-      <c r="AF25" s="186"/>
-      <c r="AG25" s="187"/>
+      <c r="AD25" s="183"/>
+      <c r="AE25" s="184"/>
+      <c r="AF25" s="184"/>
+      <c r="AG25" s="185"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
@@ -9456,10 +9671,10 @@
       <c r="AA26" s="25"/>
       <c r="AB26" s="26"/>
       <c r="AC26" s="25"/>
-      <c r="AD26" s="185"/>
-      <c r="AE26" s="186"/>
-      <c r="AF26" s="186"/>
-      <c r="AG26" s="187"/>
+      <c r="AD26" s="183"/>
+      <c r="AE26" s="184"/>
+      <c r="AF26" s="184"/>
+      <c r="AG26" s="185"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
@@ -9491,10 +9706,10 @@
       <c r="AA27" s="25"/>
       <c r="AB27" s="26"/>
       <c r="AC27" s="25"/>
-      <c r="AD27" s="185"/>
-      <c r="AE27" s="186"/>
-      <c r="AF27" s="186"/>
-      <c r="AG27" s="187"/>
+      <c r="AD27" s="183"/>
+      <c r="AE27" s="184"/>
+      <c r="AF27" s="184"/>
+      <c r="AG27" s="185"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
@@ -9526,10 +9741,10 @@
       <c r="AA28" s="25"/>
       <c r="AB28" s="26"/>
       <c r="AC28" s="25"/>
-      <c r="AD28" s="185"/>
-      <c r="AE28" s="186"/>
-      <c r="AF28" s="186"/>
-      <c r="AG28" s="187"/>
+      <c r="AD28" s="183"/>
+      <c r="AE28" s="184"/>
+      <c r="AF28" s="184"/>
+      <c r="AG28" s="185"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
@@ -9561,10 +9776,10 @@
       <c r="AA29" s="25"/>
       <c r="AB29" s="26"/>
       <c r="AC29" s="25"/>
-      <c r="AD29" s="185"/>
-      <c r="AE29" s="186"/>
-      <c r="AF29" s="186"/>
-      <c r="AG29" s="187"/>
+      <c r="AD29" s="183"/>
+      <c r="AE29" s="184"/>
+      <c r="AF29" s="184"/>
+      <c r="AG29" s="185"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
@@ -9596,10 +9811,10 @@
       <c r="AA30" s="25"/>
       <c r="AB30" s="26"/>
       <c r="AC30" s="25"/>
-      <c r="AD30" s="185"/>
-      <c r="AE30" s="186"/>
-      <c r="AF30" s="186"/>
-      <c r="AG30" s="187"/>
+      <c r="AD30" s="183"/>
+      <c r="AE30" s="184"/>
+      <c r="AF30" s="184"/>
+      <c r="AG30" s="185"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
@@ -9631,10 +9846,10 @@
       <c r="AA31" s="25"/>
       <c r="AB31" s="26"/>
       <c r="AC31" s="25"/>
-      <c r="AD31" s="185"/>
-      <c r="AE31" s="186"/>
-      <c r="AF31" s="186"/>
-      <c r="AG31" s="187"/>
+      <c r="AD31" s="183"/>
+      <c r="AE31" s="184"/>
+      <c r="AF31" s="184"/>
+      <c r="AG31" s="185"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
@@ -9666,10 +9881,10 @@
       <c r="AA32" s="25"/>
       <c r="AB32" s="26"/>
       <c r="AC32" s="25"/>
-      <c r="AD32" s="185"/>
-      <c r="AE32" s="186"/>
-      <c r="AF32" s="186"/>
-      <c r="AG32" s="187"/>
+      <c r="AD32" s="183"/>
+      <c r="AE32" s="184"/>
+      <c r="AF32" s="184"/>
+      <c r="AG32" s="185"/>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
@@ -9701,10 +9916,10 @@
       <c r="AA33" s="25"/>
       <c r="AB33" s="26"/>
       <c r="AC33" s="25"/>
-      <c r="AD33" s="185"/>
-      <c r="AE33" s="186"/>
-      <c r="AF33" s="186"/>
-      <c r="AG33" s="187"/>
+      <c r="AD33" s="183"/>
+      <c r="AE33" s="184"/>
+      <c r="AF33" s="184"/>
+      <c r="AG33" s="185"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
@@ -9736,10 +9951,10 @@
       <c r="AA34" s="25"/>
       <c r="AB34" s="26"/>
       <c r="AC34" s="25"/>
-      <c r="AD34" s="185"/>
-      <c r="AE34" s="186"/>
-      <c r="AF34" s="186"/>
-      <c r="AG34" s="187"/>
+      <c r="AD34" s="183"/>
+      <c r="AE34" s="184"/>
+      <c r="AF34" s="184"/>
+      <c r="AG34" s="185"/>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
@@ -9771,10 +9986,10 @@
       <c r="AA35" s="25"/>
       <c r="AB35" s="26"/>
       <c r="AC35" s="25"/>
-      <c r="AD35" s="185"/>
-      <c r="AE35" s="186"/>
-      <c r="AF35" s="186"/>
-      <c r="AG35" s="187"/>
+      <c r="AD35" s="183"/>
+      <c r="AE35" s="184"/>
+      <c r="AF35" s="184"/>
+      <c r="AG35" s="185"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
@@ -9806,10 +10021,10 @@
       <c r="AA36" s="25"/>
       <c r="AB36" s="26"/>
       <c r="AC36" s="25"/>
-      <c r="AD36" s="185"/>
-      <c r="AE36" s="186"/>
-      <c r="AF36" s="186"/>
-      <c r="AG36" s="187"/>
+      <c r="AD36" s="183"/>
+      <c r="AE36" s="184"/>
+      <c r="AF36" s="184"/>
+      <c r="AG36" s="185"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
@@ -9841,10 +10056,10 @@
       <c r="AA37" s="25"/>
       <c r="AB37" s="26"/>
       <c r="AC37" s="25"/>
-      <c r="AD37" s="185"/>
-      <c r="AE37" s="186"/>
-      <c r="AF37" s="186"/>
-      <c r="AG37" s="187"/>
+      <c r="AD37" s="183"/>
+      <c r="AE37" s="184"/>
+      <c r="AF37" s="184"/>
+      <c r="AG37" s="185"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
@@ -9876,10 +10091,10 @@
       <c r="AA38" s="25"/>
       <c r="AB38" s="26"/>
       <c r="AC38" s="25"/>
-      <c r="AD38" s="185"/>
-      <c r="AE38" s="186"/>
-      <c r="AF38" s="186"/>
-      <c r="AG38" s="187"/>
+      <c r="AD38" s="183"/>
+      <c r="AE38" s="184"/>
+      <c r="AF38" s="184"/>
+      <c r="AG38" s="185"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
@@ -9911,10 +10126,10 @@
       <c r="AA39" s="25"/>
       <c r="AB39" s="26"/>
       <c r="AC39" s="25"/>
-      <c r="AD39" s="185"/>
-      <c r="AE39" s="186"/>
-      <c r="AF39" s="186"/>
-      <c r="AG39" s="187"/>
+      <c r="AD39" s="183"/>
+      <c r="AE39" s="184"/>
+      <c r="AF39" s="184"/>
+      <c r="AG39" s="185"/>
     </row>
     <row r="40" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="52"/>
@@ -9946,35 +10161,32 @@
       <c r="AA40" s="38"/>
       <c r="AB40" s="39"/>
       <c r="AC40" s="38"/>
-      <c r="AD40" s="182"/>
-      <c r="AE40" s="183"/>
-      <c r="AF40" s="183"/>
-      <c r="AG40" s="184"/>
+      <c r="AD40" s="193"/>
+      <c r="AE40" s="194"/>
+      <c r="AF40" s="194"/>
+      <c r="AG40" s="195"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AD5:AG5"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AG3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="AD40:AG40"/>
+    <mergeCell ref="AD34:AG34"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AD36:AG36"/>
+    <mergeCell ref="AD37:AG37"/>
+    <mergeCell ref="AD38:AG38"/>
+    <mergeCell ref="AD39:AG39"/>
+    <mergeCell ref="AD33:AG33"/>
+    <mergeCell ref="AD22:AG22"/>
+    <mergeCell ref="AD23:AG23"/>
+    <mergeCell ref="AD24:AG24"/>
+    <mergeCell ref="AD25:AG25"/>
+    <mergeCell ref="AD26:AG26"/>
+    <mergeCell ref="AD27:AG27"/>
+    <mergeCell ref="AD28:AG28"/>
+    <mergeCell ref="AD29:AG29"/>
+    <mergeCell ref="AD30:AG30"/>
+    <mergeCell ref="AD31:AG31"/>
+    <mergeCell ref="AD32:AG32"/>
     <mergeCell ref="AD7:AG7"/>
     <mergeCell ref="AD8:AG8"/>
     <mergeCell ref="AD21:AG21"/>
@@ -9990,25 +10202,28 @@
     <mergeCell ref="AD19:AG19"/>
     <mergeCell ref="AD20:AG20"/>
     <mergeCell ref="AD9:AG9"/>
-    <mergeCell ref="AD33:AG33"/>
-    <mergeCell ref="AD22:AG22"/>
-    <mergeCell ref="AD23:AG23"/>
-    <mergeCell ref="AD24:AG24"/>
-    <mergeCell ref="AD25:AG25"/>
-    <mergeCell ref="AD26:AG26"/>
-    <mergeCell ref="AD27:AG27"/>
-    <mergeCell ref="AD28:AG28"/>
-    <mergeCell ref="AD29:AG29"/>
-    <mergeCell ref="AD30:AG30"/>
-    <mergeCell ref="AD31:AG31"/>
-    <mergeCell ref="AD32:AG32"/>
-    <mergeCell ref="AD40:AG40"/>
-    <mergeCell ref="AD34:AG34"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AD36:AG36"/>
-    <mergeCell ref="AD37:AG37"/>
-    <mergeCell ref="AD38:AG38"/>
-    <mergeCell ref="AD39:AG39"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AD5:AG5"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AG3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bad Input" error="Input for this cell must be one of the listed types and all uppercase!" sqref="O4:O40">

</xml_diff>